<commit_message>
Correction on hydrocarbon synthesis efficiency and typo
</commit_message>
<xml_diff>
--- a/aeromaps/resources/energy_data/hydrogen_and_electrofuel.xlsx
+++ b/aeromaps/resources/energy_data/hydrogen_and_electrofuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.fabre.ISAE-SUPAERO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.salgas.ISAE-SUPAERO\PycharmProjects\AeroMAPS\aeromaps\resources\energy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DCD479-D2C7-410B-937F-AAE427ADD485}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA84426-C611-4801-B0DC-8B8DE52BE690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{038806FC-4710-4213-AEBF-AE02FE7EEF14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{038806FC-4710-4213-AEBF-AE02FE7EEF14}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthesis" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
   <si>
     <t>Reference number</t>
   </si>
@@ -431,6 +442,9 @@
   </si>
   <si>
     <t>Q3 envelope</t>
+  </si>
+  <si>
+    <t>Modified from 0.4 of [9]to remove transport and distribution losses.</t>
   </si>
 </sst>
 </file>
@@ -440,7 +454,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1499,168 +1513,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1670,49 +1528,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
@@ -1731,6 +1571,180 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3901,7 +3915,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3933,7 +3947,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1338112640"/>
@@ -4009,7 +4023,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4041,7 +4055,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1899393152"/>
@@ -4086,7 +4100,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5253,7 +5267,7 @@
               </a:r>
               <a:r>
                 <a:rPr lang="fr-FR" sz="1100"/>
-                <a:t> = 0.4</a:t>
+                <a:t> =0,44</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5367,7 +5381,7 @@
                     <a:srgbClr val="FF0000"/>
                   </a:solidFill>
                 </a:rPr>
-                <a:t> = 0.67</a:t>
+                <a:t> = 0.74</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5744,212 +5758,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="106"/>
-      <c r="K1" s="121" t="s">
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="141"/>
+      <c r="K1" s="153" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="123"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="155"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="107"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="109"/>
+      <c r="A2" s="142"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="144"/>
       <c r="K2" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="154" t="s">
+      <c r="L2" s="156" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="154"/>
-      <c r="N2" s="155"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="157"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="112"/>
+      <c r="A3" s="145"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="147"/>
       <c r="K3" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="116" t="s">
+      <c r="L3" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="116"/>
-      <c r="N3" s="102"/>
+      <c r="M3" s="124"/>
+      <c r="N3" s="125"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="110"/>
-      <c r="B4" s="111"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="112"/>
+      <c r="A4" s="145"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="147"/>
       <c r="K4" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="116" t="s">
+      <c r="L4" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="116"/>
-      <c r="N4" s="102"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="125"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="110"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="112"/>
+      <c r="A5" s="145"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="147"/>
       <c r="K5" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="116" t="s">
+      <c r="L5" s="124" t="s">
         <v>88</v>
       </c>
-      <c r="M5" s="116"/>
-      <c r="N5" s="102"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="125"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="110"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="112"/>
+      <c r="A6" s="145"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="147"/>
       <c r="K6" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="L6" s="116" t="s">
+      <c r="L6" s="124" t="s">
         <v>90</v>
       </c>
-      <c r="M6" s="116"/>
-      <c r="N6" s="102"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="125"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="110"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="112"/>
+      <c r="A7" s="145"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="147"/>
       <c r="K7" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="117" t="s">
+      <c r="L7" s="137" t="s">
         <v>96</v>
       </c>
-      <c r="M7" s="118"/>
-      <c r="N7" s="119"/>
+      <c r="M7" s="138"/>
+      <c r="N7" s="132"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="110"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="112"/>
+      <c r="A8" s="145"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="147"/>
       <c r="K8" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="L8" s="117" t="s">
+      <c r="L8" s="137" t="s">
         <v>97</v>
       </c>
-      <c r="M8" s="118"/>
-      <c r="N8" s="119"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="132"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="110"/>
-      <c r="B9" s="111"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="112"/>
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="146"/>
+      <c r="D9" s="146"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="147"/>
       <c r="K9" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="L9" s="116" t="s">
+      <c r="L9" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="116"/>
-      <c r="N9" s="102"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="125"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="111"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="112"/>
+      <c r="A10" s="145"/>
+      <c r="B10" s="146"/>
+      <c r="C10" s="146"/>
+      <c r="D10" s="146"/>
+      <c r="E10" s="146"/>
+      <c r="F10" s="147"/>
       <c r="K10" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="L10" s="117" t="s">
+      <c r="L10" s="137" t="s">
         <v>124</v>
       </c>
-      <c r="M10" s="118"/>
-      <c r="N10" s="119"/>
+      <c r="M10" s="138"/>
+      <c r="N10" s="132"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="112"/>
+      <c r="A11" s="145"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="146"/>
+      <c r="D11" s="146"/>
+      <c r="E11" s="146"/>
+      <c r="F11" s="147"/>
       <c r="K11" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="L11" s="116" t="s">
+      <c r="L11" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="M11" s="116"/>
-      <c r="N11" s="102"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="125"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="110"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="112"/>
+      <c r="A12" s="145"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="147"/>
       <c r="K12" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="116" t="s">
+      <c r="L12" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="116"/>
-      <c r="N12" s="102"/>
+      <c r="M12" s="124"/>
+      <c r="N12" s="125"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
-      <c r="B13" s="114"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="115"/>
+      <c r="A13" s="148"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="149"/>
+      <c r="D13" s="149"/>
+      <c r="E13" s="149"/>
+      <c r="F13" s="150"/>
       <c r="K13" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="116" t="s">
+      <c r="L13" s="124" t="s">
         <v>79</v>
       </c>
-      <c r="M13" s="116"/>
-      <c r="N13" s="102"/>
+      <c r="M13" s="124"/>
+      <c r="N13" s="125"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="77"/>
@@ -5961,11 +5975,11 @@
       <c r="K14" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="L14" s="120" t="s">
+      <c r="L14" s="151" t="s">
         <v>81</v>
       </c>
-      <c r="M14" s="120"/>
-      <c r="N14" s="103"/>
+      <c r="M14" s="151"/>
+      <c r="N14" s="152"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="77"/>
@@ -5998,32 +6012,32 @@
       <c r="N17" s="57"/>
     </row>
     <row r="18" spans="1:14" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="142" t="s">
+      <c r="A18" s="126" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="144"/>
+      <c r="B18" s="128"/>
       <c r="C18" s="57"/>
-      <c r="D18" s="142" t="s">
+      <c r="D18" s="126" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="144"/>
-      <c r="I18" s="142" t="s">
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="128"/>
+      <c r="I18" s="126" t="s">
         <v>105</v>
       </c>
-      <c r="J18" s="143"/>
-      <c r="K18" s="144"/>
-      <c r="M18" s="142" t="s">
+      <c r="J18" s="127"/>
+      <c r="K18" s="128"/>
+      <c r="M18" s="126" t="s">
         <v>118</v>
       </c>
-      <c r="N18" s="144"/>
+      <c r="N18" s="128"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="157" t="s">
+      <c r="B19" s="105" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="81" t="s">
@@ -6035,14 +6049,14 @@
       <c r="F19" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="156" t="s">
+      <c r="G19" s="104" t="s">
         <v>51</v>
       </c>
       <c r="I19" s="83"/>
-      <c r="J19" s="152" t="s">
+      <c r="J19" s="135" t="s">
         <v>106</v>
       </c>
-      <c r="K19" s="153"/>
+      <c r="K19" s="136"/>
       <c r="M19" s="94" t="s">
         <v>117</v>
       </c>
@@ -6054,7 +6068,7 @@
       <c r="A20" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="158">
+      <c r="B20" s="106">
         <f>'H2 Efficiency'!E3</f>
         <v>0.58499999999999996</v>
       </c>
@@ -6076,11 +6090,11 @@
       <c r="I20" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="J20" s="150">
+      <c r="J20" s="133">
         <f>'H2 Emission factors'!C55</f>
         <v>5.8012791572610987E-2</v>
       </c>
-      <c r="K20" s="151"/>
+      <c r="K20" s="134"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="82"/>
@@ -6104,11 +6118,11 @@
       <c r="I21" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="J21" s="149">
+      <c r="J21" s="131">
         <f>'H2 Emission factors'!D55</f>
         <v>6.5621733887176736E-2</v>
       </c>
-      <c r="K21" s="119"/>
+      <c r="K21" s="132"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="82"/>
@@ -6132,11 +6146,11 @@
       <c r="I22" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="J22" s="147">
+      <c r="J22" s="129">
         <f>'H2 Emission factors'!E55</f>
         <v>8.673913043478261E-2</v>
       </c>
-      <c r="K22" s="148"/>
+      <c r="K22" s="130"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="79" t="s">
@@ -6146,11 +6160,11 @@
         <f>'H2 Emission factors'!B6</f>
         <v>2.1</v>
       </c>
-      <c r="F23" s="145">
+      <c r="F23" s="102">
         <f>'H2 Emission factors'!C6</f>
         <v>4.87</v>
       </c>
-      <c r="G23" s="146">
+      <c r="G23" s="103">
         <f>'H2 Emission factors'!D6</f>
         <v>6.2</v>
       </c>
@@ -6167,15 +6181,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L10:N10"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F13"/>
     <mergeCell ref="L5:N5"/>
@@ -6186,10 +6191,19 @@
     <mergeCell ref="L13:N13"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L14:N14"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L14:N14"/>
     <mergeCell ref="M18:N18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6218,18 +6232,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="158" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="128"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="160"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
@@ -6296,11 +6310,11 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="129" t="s">
+      <c r="A6" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="130"/>
-      <c r="C6" s="131"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
     </row>
@@ -6394,7 +6408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA1880-BBB6-450E-9F9A-6C01F7F0B90B}">
   <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
@@ -6411,14 +6425,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="175" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="141"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="177"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
@@ -6558,18 +6572,18 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="159" t="s">
+      <c r="A8" s="170" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="160"/>
-      <c r="C8" s="160"/>
-      <c r="D8" s="160"/>
-      <c r="E8" s="160"/>
-      <c r="F8" s="160"/>
-      <c r="G8" s="160"/>
-      <c r="H8" s="160"/>
-      <c r="I8" s="160"/>
-      <c r="J8" s="161"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="171"/>
+      <c r="D8" s="171"/>
+      <c r="E8" s="171"/>
+      <c r="F8" s="171"/>
+      <c r="G8" s="171"/>
+      <c r="H8" s="171"/>
+      <c r="I8" s="171"/>
+      <c r="J8" s="172"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="57"/>
@@ -6732,23 +6746,23 @@
       <c r="G23" s="29"/>
     </row>
     <row r="24" spans="1:11" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="173" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="125"/>
+      <c r="B24" s="174"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="124" t="s">
+      <c r="D24" s="173" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="125"/>
-      <c r="G24" s="124" t="s">
+      <c r="E24" s="174"/>
+      <c r="G24" s="173" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="125"/>
-      <c r="J24" s="124" t="s">
+      <c r="H24" s="174"/>
+      <c r="J24" s="173" t="s">
         <v>64</v>
       </c>
-      <c r="K24" s="125"/>
+      <c r="K24" s="174"/>
     </row>
     <row r="25" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="51" t="s">
@@ -6909,12 +6923,12 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="132" t="s">
+      <c r="A35" s="167" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="133"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="134"/>
+      <c r="B35" s="168"/>
+      <c r="C35" s="168"/>
+      <c r="D35" s="169"/>
     </row>
     <row r="36" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="58" t="s">
@@ -7100,37 +7114,37 @@
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="166" t="s">
+      <c r="A52" s="164" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="167"/>
-      <c r="C52" s="167"/>
-      <c r="D52" s="167"/>
-      <c r="E52" s="168"/>
+      <c r="B52" s="165"/>
+      <c r="C52" s="165"/>
+      <c r="D52" s="165"/>
+      <c r="E52" s="166"/>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="176" t="s">
+      <c r="A53" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="179"/>
-      <c r="C53" s="178" t="s">
+      <c r="B53" s="121"/>
+      <c r="C53" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="175" t="s">
+      <c r="D53" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="E53" s="177" t="s">
+      <c r="E53" s="119" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="165">
-        <f>D37/C37</f>
+      <c r="A54" s="110">
+        <f t="shared" ref="A54:A65" si="0">D37/C37</f>
         <v>0.17391304347826086</v>
       </c>
-      <c r="B54" s="180"/>
+      <c r="B54" s="122"/>
       <c r="C54" s="75" t="s">
         <v>129</v>
       </c>
@@ -7142,240 +7156,240 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="162">
-        <f>D38/C38</f>
+      <c r="A55" s="107">
+        <f t="shared" si="0"/>
         <v>9.3913043478260877E-2</v>
       </c>
-      <c r="B55" s="181"/>
-      <c r="C55" s="164">
+      <c r="B55" s="123"/>
+      <c r="C55" s="109">
         <f>QUARTILE(A54:A65,1)</f>
         <v>5.8012791572610987E-2</v>
       </c>
-      <c r="D55" s="164">
+      <c r="D55" s="109">
         <f>MEDIAN(A54:A65)</f>
         <v>6.5621733887176736E-2</v>
       </c>
-      <c r="E55" s="172">
+      <c r="E55" s="114">
         <f>QUARTILE(A54:A65,3)</f>
         <v>8.673913043478261E-2</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="163">
-        <f>D39/C39</f>
+      <c r="A56" s="108">
+        <f t="shared" si="0"/>
         <v>6.08695652173913E-2</v>
       </c>
-      <c r="B56" s="166" t="s">
+      <c r="B56" s="164" t="s">
         <v>131</v>
       </c>
-      <c r="C56" s="167"/>
-      <c r="D56" s="167"/>
-      <c r="E56" s="168"/>
+      <c r="C56" s="165"/>
+      <c r="D56" s="165"/>
+      <c r="E56" s="166"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="163">
-        <f>D40/C40</f>
+      <c r="A57" s="108">
+        <f t="shared" si="0"/>
         <v>8.4347826086956526E-2</v>
       </c>
       <c r="B57" s="34">
         <v>0</v>
       </c>
-      <c r="C57" s="165">
-        <f>$C$55*B57</f>
+      <c r="C57" s="110">
+        <f t="shared" ref="C57:C88" si="1">$C$55*B57</f>
         <v>0</v>
       </c>
-      <c r="D57" s="165">
-        <f>$D$55*B57</f>
+      <c r="D57" s="110">
+        <f t="shared" ref="D57:D88" si="2">$D$55*B57</f>
         <v>0</v>
       </c>
-      <c r="E57" s="169">
-        <f>$E$55*B57</f>
+      <c r="E57" s="111">
+        <f t="shared" ref="E57:E88" si="3">$E$55*B57</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="163">
-        <f>D41/C41</f>
+      <c r="A58" s="108">
+        <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="B58" s="31">
         <v>5</v>
       </c>
-      <c r="C58" s="162">
-        <f>$C$55*B58</f>
+      <c r="C58" s="107">
+        <f t="shared" si="1"/>
         <v>0.29006395786305494</v>
       </c>
-      <c r="D58" s="162">
-        <f>$D$55*B58</f>
+      <c r="D58" s="107">
+        <f t="shared" si="2"/>
         <v>0.32810866943588368</v>
       </c>
-      <c r="E58" s="170">
-        <f>$E$55*B58</f>
+      <c r="E58" s="112">
+        <f t="shared" si="3"/>
         <v>0.43369565217391304</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="163">
-        <f>D42/C42</f>
+      <c r="A59" s="108">
+        <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="B59" s="31">
         <v>10</v>
       </c>
-      <c r="C59" s="162">
-        <f>$C$55*B59</f>
+      <c r="C59" s="107">
+        <f t="shared" si="1"/>
         <v>0.58012791572610989</v>
       </c>
-      <c r="D59" s="162">
-        <f>$D$55*B59</f>
+      <c r="D59" s="107">
+        <f t="shared" si="2"/>
         <v>0.65621733887176736</v>
       </c>
-      <c r="E59" s="170">
-        <f>$E$55*B59</f>
+      <c r="E59" s="112">
+        <f t="shared" si="3"/>
         <v>0.86739130434782608</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="163">
-        <f>D43/C43</f>
+      <c r="A60" s="108">
+        <f t="shared" si="0"/>
         <v>4.0444444444444443E-2</v>
       </c>
       <c r="B60" s="31">
         <v>15</v>
       </c>
-      <c r="C60" s="162">
-        <f>$C$55*B60</f>
+      <c r="C60" s="107">
+        <f t="shared" si="1"/>
         <v>0.87019187358916483</v>
       </c>
-      <c r="D60" s="162">
-        <f>$D$55*B60</f>
+      <c r="D60" s="107">
+        <f t="shared" si="2"/>
         <v>0.98432600830765105</v>
       </c>
-      <c r="E60" s="170">
-        <f>$E$55*B60</f>
+      <c r="E60" s="112">
+        <f t="shared" si="3"/>
         <v>1.3010869565217391</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="163">
-        <f>D44/C44</f>
+      <c r="A61" s="108">
+        <f t="shared" si="0"/>
         <v>5.7333333333333333E-2</v>
       </c>
       <c r="B61" s="31">
         <v>20</v>
       </c>
-      <c r="C61" s="162">
-        <f>$C$55*B61</f>
+      <c r="C61" s="107">
+        <f t="shared" si="1"/>
         <v>1.1602558314522198</v>
       </c>
-      <c r="D61" s="162">
-        <f>$D$55*B61</f>
+      <c r="D61" s="107">
+        <f t="shared" si="2"/>
         <v>1.3124346777435347</v>
       </c>
-      <c r="E61" s="170">
-        <f>$E$55*B61</f>
+      <c r="E61" s="112">
+        <f t="shared" si="3"/>
         <v>1.7347826086956522</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="163">
-        <f>D45/C45</f>
+      <c r="A62" s="108">
+        <f t="shared" si="0"/>
         <v>9.451219512195122E-2</v>
       </c>
       <c r="B62" s="31">
         <v>25</v>
       </c>
-      <c r="C62" s="162">
-        <f>$C$55*B62</f>
+      <c r="C62" s="107">
+        <f t="shared" si="1"/>
         <v>1.4503197893152746</v>
       </c>
-      <c r="D62" s="162">
-        <f>$D$55*B62</f>
+      <c r="D62" s="107">
+        <f t="shared" si="2"/>
         <v>1.6405433471794184</v>
       </c>
-      <c r="E62" s="170">
-        <f>$E$55*B62</f>
+      <c r="E62" s="112">
+        <f t="shared" si="3"/>
         <v>2.1684782608695654</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="163">
-        <f>D46/C46</f>
+      <c r="A63" s="108">
+        <f t="shared" si="0"/>
         <v>6.6537585421412304E-2</v>
       </c>
       <c r="B63" s="31">
         <v>30</v>
       </c>
-      <c r="C63" s="162">
-        <f>$C$55*B63</f>
+      <c r="C63" s="107">
+        <f t="shared" si="1"/>
         <v>1.7403837471783297</v>
       </c>
-      <c r="D63" s="162">
-        <f>$D$55*B63</f>
+      <c r="D63" s="107">
+        <f t="shared" si="2"/>
         <v>1.9686520166153021</v>
       </c>
-      <c r="E63" s="170">
-        <f>$E$55*B63</f>
+      <c r="E63" s="112">
+        <f t="shared" si="3"/>
         <v>2.6021739130434782</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="163">
-        <f>D47/C47</f>
+      <c r="A64" s="108">
+        <f t="shared" si="0"/>
         <v>6.4705882352941183E-2</v>
       </c>
       <c r="B64" s="31">
         <v>35</v>
       </c>
-      <c r="C64" s="162">
-        <f>$C$55*B64</f>
+      <c r="C64" s="107">
+        <f t="shared" si="1"/>
         <v>2.0304477050413845</v>
       </c>
-      <c r="D64" s="162">
-        <f>$D$55*B64</f>
+      <c r="D64" s="107">
+        <f t="shared" si="2"/>
         <v>2.2967606860511856</v>
       </c>
-      <c r="E64" s="170">
-        <f>$E$55*B64</f>
+      <c r="E64" s="112">
+        <f t="shared" si="3"/>
         <v>3.0358695652173915</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="173">
-        <f>D48/C48</f>
+      <c r="A65" s="115">
+        <f t="shared" si="0"/>
         <v>5.8239277652370205E-2</v>
       </c>
       <c r="B65" s="31">
         <v>40</v>
       </c>
-      <c r="C65" s="162">
-        <f>$C$55*B65</f>
+      <c r="C65" s="107">
+        <f t="shared" si="1"/>
         <v>2.3205116629044396</v>
       </c>
-      <c r="D65" s="162">
-        <f>$D$55*B65</f>
+      <c r="D65" s="107">
+        <f t="shared" si="2"/>
         <v>2.6248693554870695</v>
       </c>
-      <c r="E65" s="170">
-        <f>$E$55*B65</f>
+      <c r="E65" s="112">
+        <f t="shared" si="3"/>
         <v>3.4695652173913043</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="174"/>
+      <c r="A66" s="116"/>
       <c r="B66" s="31">
         <v>45</v>
       </c>
-      <c r="C66" s="162">
-        <f>$C$55*B66</f>
+      <c r="C66" s="107">
+        <f t="shared" si="1"/>
         <v>2.6105756207674946</v>
       </c>
-      <c r="D66" s="162">
-        <f>$D$55*B66</f>
+      <c r="D66" s="107">
+        <f t="shared" si="2"/>
         <v>2.9529780249229534</v>
       </c>
-      <c r="E66" s="170">
-        <f>$E$55*B66</f>
+      <c r="E66" s="112">
+        <f t="shared" si="3"/>
         <v>3.9032608695652176</v>
       </c>
     </row>
@@ -7383,16 +7397,16 @@
       <c r="B67" s="31">
         <v>50</v>
       </c>
-      <c r="C67" s="162">
-        <f>$C$55*B67</f>
+      <c r="C67" s="107">
+        <f t="shared" si="1"/>
         <v>2.9006395786305492</v>
       </c>
-      <c r="D67" s="162">
-        <f>$D$55*B67</f>
+      <c r="D67" s="107">
+        <f t="shared" si="2"/>
         <v>3.2810866943588368</v>
       </c>
-      <c r="E67" s="170">
-        <f>$E$55*B67</f>
+      <c r="E67" s="112">
+        <f t="shared" si="3"/>
         <v>4.3369565217391308</v>
       </c>
     </row>
@@ -7400,16 +7414,16 @@
       <c r="B68" s="31">
         <v>55</v>
       </c>
-      <c r="C68" s="162">
-        <f>$C$55*B68</f>
+      <c r="C68" s="107">
+        <f t="shared" si="1"/>
         <v>3.1907035364936043</v>
       </c>
-      <c r="D68" s="162">
-        <f>$D$55*B68</f>
+      <c r="D68" s="107">
+        <f t="shared" si="2"/>
         <v>3.6091953637947203</v>
       </c>
-      <c r="E68" s="170">
-        <f>$E$55*B68</f>
+      <c r="E68" s="112">
+        <f t="shared" si="3"/>
         <v>4.7706521739130432</v>
       </c>
     </row>
@@ -7417,16 +7431,16 @@
       <c r="B69" s="31">
         <v>60</v>
       </c>
-      <c r="C69" s="162">
-        <f>$C$55*B69</f>
+      <c r="C69" s="107">
+        <f t="shared" si="1"/>
         <v>3.4807674943566593</v>
       </c>
-      <c r="D69" s="162">
-        <f>$D$55*B69</f>
+      <c r="D69" s="107">
+        <f t="shared" si="2"/>
         <v>3.9373040332306042</v>
       </c>
-      <c r="E69" s="170">
-        <f>$E$55*B69</f>
+      <c r="E69" s="112">
+        <f t="shared" si="3"/>
         <v>5.2043478260869565</v>
       </c>
     </row>
@@ -7434,16 +7448,16 @@
       <c r="B70" s="31">
         <v>65</v>
       </c>
-      <c r="C70" s="162">
-        <f>$C$55*B70</f>
+      <c r="C70" s="107">
+        <f t="shared" si="1"/>
         <v>3.7708314522197144</v>
       </c>
-      <c r="D70" s="162">
-        <f>$D$55*B70</f>
+      <c r="D70" s="107">
+        <f t="shared" si="2"/>
         <v>4.2654127026664881</v>
       </c>
-      <c r="E70" s="170">
-        <f>$E$55*B70</f>
+      <c r="E70" s="112">
+        <f t="shared" si="3"/>
         <v>5.6380434782608697</v>
       </c>
     </row>
@@ -7451,16 +7465,16 @@
       <c r="B71" s="31">
         <v>70</v>
       </c>
-      <c r="C71" s="162">
-        <f>$C$55*B71</f>
+      <c r="C71" s="107">
+        <f t="shared" si="1"/>
         <v>4.060895410082769</v>
       </c>
-      <c r="D71" s="162">
-        <f>$D$55*B71</f>
+      <c r="D71" s="107">
+        <f t="shared" si="2"/>
         <v>4.5935213721023711</v>
       </c>
-      <c r="E71" s="170">
-        <f>$E$55*B71</f>
+      <c r="E71" s="112">
+        <f t="shared" si="3"/>
         <v>6.071739130434783</v>
       </c>
     </row>
@@ -7468,16 +7482,16 @@
       <c r="B72" s="31">
         <v>75</v>
       </c>
-      <c r="C72" s="162">
-        <f>$C$55*B72</f>
+      <c r="C72" s="107">
+        <f t="shared" si="1"/>
         <v>4.3509593679458245</v>
       </c>
-      <c r="D72" s="162">
-        <f>$D$55*B72</f>
+      <c r="D72" s="107">
+        <f t="shared" si="2"/>
         <v>4.921630041538255</v>
       </c>
-      <c r="E72" s="170">
-        <f>$E$55*B72</f>
+      <c r="E72" s="112">
+        <f t="shared" si="3"/>
         <v>6.5054347826086953</v>
       </c>
     </row>
@@ -7485,16 +7499,16 @@
       <c r="B73" s="31">
         <v>80</v>
       </c>
-      <c r="C73" s="162">
-        <f>$C$55*B73</f>
+      <c r="C73" s="107">
+        <f t="shared" si="1"/>
         <v>4.6410233258088791</v>
       </c>
-      <c r="D73" s="162">
-        <f>$D$55*B73</f>
+      <c r="D73" s="107">
+        <f t="shared" si="2"/>
         <v>5.2497387109741389</v>
       </c>
-      <c r="E73" s="170">
-        <f>$E$55*B73</f>
+      <c r="E73" s="112">
+        <f t="shared" si="3"/>
         <v>6.9391304347826086</v>
       </c>
     </row>
@@ -7502,16 +7516,16 @@
       <c r="B74" s="31">
         <v>85</v>
       </c>
-      <c r="C74" s="162">
-        <f>$C$55*B74</f>
+      <c r="C74" s="107">
+        <f t="shared" si="1"/>
         <v>4.9310872836719337</v>
       </c>
-      <c r="D74" s="162">
-        <f>$D$55*B74</f>
+      <c r="D74" s="107">
+        <f t="shared" si="2"/>
         <v>5.5778473804100228</v>
       </c>
-      <c r="E74" s="170">
-        <f>$E$55*B74</f>
+      <c r="E74" s="112">
+        <f t="shared" si="3"/>
         <v>7.3728260869565219</v>
       </c>
     </row>
@@ -7519,16 +7533,16 @@
       <c r="B75" s="31">
         <v>90</v>
       </c>
-      <c r="C75" s="162">
-        <f>$C$55*B75</f>
+      <c r="C75" s="107">
+        <f t="shared" si="1"/>
         <v>5.2211512415349892</v>
       </c>
-      <c r="D75" s="162">
-        <f>$D$55*B75</f>
+      <c r="D75" s="107">
+        <f t="shared" si="2"/>
         <v>5.9059560498459067</v>
       </c>
-      <c r="E75" s="170">
-        <f>$E$55*B75</f>
+      <c r="E75" s="112">
+        <f t="shared" si="3"/>
         <v>7.8065217391304351</v>
       </c>
     </row>
@@ -7536,16 +7550,16 @@
       <c r="B76" s="31">
         <v>95</v>
       </c>
-      <c r="C76" s="162">
-        <f>$C$55*B76</f>
+      <c r="C76" s="107">
+        <f t="shared" si="1"/>
         <v>5.5112151993980438</v>
       </c>
-      <c r="D76" s="162">
-        <f>$D$55*B76</f>
+      <c r="D76" s="107">
+        <f t="shared" si="2"/>
         <v>6.2340647192817897</v>
       </c>
-      <c r="E76" s="170">
-        <f>$E$55*B76</f>
+      <c r="E76" s="112">
+        <f t="shared" si="3"/>
         <v>8.2402173913043484</v>
       </c>
     </row>
@@ -7553,16 +7567,16 @@
       <c r="B77" s="31">
         <v>100</v>
       </c>
-      <c r="C77" s="162">
-        <f>$C$55*B77</f>
+      <c r="C77" s="107">
+        <f t="shared" si="1"/>
         <v>5.8012791572610984</v>
       </c>
-      <c r="D77" s="162">
-        <f>$D$55*B77</f>
+      <c r="D77" s="107">
+        <f t="shared" si="2"/>
         <v>6.5621733887176736</v>
       </c>
-      <c r="E77" s="170">
-        <f>$E$55*B77</f>
+      <c r="E77" s="112">
+        <f t="shared" si="3"/>
         <v>8.6739130434782616</v>
       </c>
     </row>
@@ -7570,16 +7584,16 @@
       <c r="B78" s="31">
         <v>105</v>
       </c>
-      <c r="C78" s="162">
-        <f>$C$55*B78</f>
+      <c r="C78" s="107">
+        <f t="shared" si="1"/>
         <v>6.0913431151241539</v>
       </c>
-      <c r="D78" s="162">
-        <f>$D$55*B78</f>
+      <c r="D78" s="107">
+        <f t="shared" si="2"/>
         <v>6.8902820581535575</v>
       </c>
-      <c r="E78" s="170">
-        <f>$E$55*B78</f>
+      <c r="E78" s="112">
+        <f t="shared" si="3"/>
         <v>9.1076086956521749</v>
       </c>
     </row>
@@ -7587,16 +7601,16 @@
       <c r="B79" s="31">
         <v>110</v>
       </c>
-      <c r="C79" s="162">
-        <f>$C$55*B79</f>
+      <c r="C79" s="107">
+        <f t="shared" si="1"/>
         <v>6.3814070729872086</v>
       </c>
-      <c r="D79" s="162">
-        <f>$D$55*B79</f>
+      <c r="D79" s="107">
+        <f t="shared" si="2"/>
         <v>7.2183907275894406</v>
       </c>
-      <c r="E79" s="170">
-        <f>$E$55*B79</f>
+      <c r="E79" s="112">
+        <f t="shared" si="3"/>
         <v>9.5413043478260864</v>
       </c>
     </row>
@@ -7604,16 +7618,16 @@
       <c r="B80" s="31">
         <v>115</v>
       </c>
-      <c r="C80" s="162">
-        <f>$C$55*B80</f>
+      <c r="C80" s="107">
+        <f t="shared" si="1"/>
         <v>6.6714710308502632</v>
       </c>
-      <c r="D80" s="162">
-        <f>$D$55*B80</f>
+      <c r="D80" s="107">
+        <f t="shared" si="2"/>
         <v>7.5464993970253245</v>
       </c>
-      <c r="E80" s="170">
-        <f>$E$55*B80</f>
+      <c r="E80" s="112">
+        <f t="shared" si="3"/>
         <v>9.9749999999999996</v>
       </c>
     </row>
@@ -7621,16 +7635,16 @@
       <c r="B81" s="31">
         <v>120</v>
       </c>
-      <c r="C81" s="162">
-        <f>$C$55*B81</f>
+      <c r="C81" s="107">
+        <f t="shared" si="1"/>
         <v>6.9615349887133187</v>
       </c>
-      <c r="D81" s="162">
-        <f>$D$55*B81</f>
+      <c r="D81" s="107">
+        <f t="shared" si="2"/>
         <v>7.8746080664612084</v>
       </c>
-      <c r="E81" s="170">
-        <f>$E$55*B81</f>
+      <c r="E81" s="112">
+        <f t="shared" si="3"/>
         <v>10.408695652173913</v>
       </c>
     </row>
@@ -7638,16 +7652,16 @@
       <c r="B82" s="31">
         <v>125</v>
       </c>
-      <c r="C82" s="162">
-        <f>$C$55*B82</f>
+      <c r="C82" s="107">
+        <f t="shared" si="1"/>
         <v>7.2515989465763733</v>
       </c>
-      <c r="D82" s="162">
-        <f>$D$55*B82</f>
+      <c r="D82" s="107">
+        <f t="shared" si="2"/>
         <v>8.2027167358970914</v>
       </c>
-      <c r="E82" s="170">
-        <f>$E$55*B82</f>
+      <c r="E82" s="112">
+        <f t="shared" si="3"/>
         <v>10.842391304347826</v>
       </c>
     </row>
@@ -7655,16 +7669,16 @@
       <c r="B83" s="31">
         <v>130</v>
       </c>
-      <c r="C83" s="162">
-        <f>$C$55*B83</f>
+      <c r="C83" s="107">
+        <f t="shared" si="1"/>
         <v>7.5416629044394288</v>
       </c>
-      <c r="D83" s="162">
-        <f>$D$55*B83</f>
+      <c r="D83" s="107">
+        <f t="shared" si="2"/>
         <v>8.5308254053329762</v>
       </c>
-      <c r="E83" s="170">
-        <f>$E$55*B83</f>
+      <c r="E83" s="112">
+        <f t="shared" si="3"/>
         <v>11.276086956521739</v>
       </c>
     </row>
@@ -7672,16 +7686,16 @@
       <c r="B84" s="31">
         <v>135</v>
       </c>
-      <c r="C84" s="162">
-        <f>$C$55*B84</f>
+      <c r="C84" s="107">
+        <f t="shared" si="1"/>
         <v>7.8317268623024834</v>
       </c>
-      <c r="D84" s="162">
-        <f>$D$55*B84</f>
+      <c r="D84" s="107">
+        <f t="shared" si="2"/>
         <v>8.8589340747688592</v>
       </c>
-      <c r="E84" s="170">
-        <f>$E$55*B84</f>
+      <c r="E84" s="112">
+        <f t="shared" si="3"/>
         <v>11.709782608695653</v>
       </c>
     </row>
@@ -7689,16 +7703,16 @@
       <c r="B85" s="31">
         <v>140</v>
       </c>
-      <c r="C85" s="162">
-        <f>$C$55*B85</f>
+      <c r="C85" s="107">
+        <f t="shared" si="1"/>
         <v>8.121790820165538</v>
       </c>
-      <c r="D85" s="162">
-        <f>$D$55*B85</f>
+      <c r="D85" s="107">
+        <f t="shared" si="2"/>
         <v>9.1870427442047422</v>
       </c>
-      <c r="E85" s="170">
-        <f>$E$55*B85</f>
+      <c r="E85" s="112">
+        <f t="shared" si="3"/>
         <v>12.143478260869566</v>
       </c>
     </row>
@@ -7706,16 +7720,16 @@
       <c r="B86" s="31">
         <v>145</v>
       </c>
-      <c r="C86" s="162">
-        <f>$C$55*B86</f>
+      <c r="C86" s="107">
+        <f t="shared" si="1"/>
         <v>8.4118547780285926</v>
       </c>
-      <c r="D86" s="162">
-        <f>$D$55*B86</f>
+      <c r="D86" s="107">
+        <f t="shared" si="2"/>
         <v>9.515151413640627</v>
       </c>
-      <c r="E86" s="170">
-        <f>$E$55*B86</f>
+      <c r="E86" s="112">
+        <f t="shared" si="3"/>
         <v>12.577173913043479</v>
       </c>
     </row>
@@ -7723,16 +7737,16 @@
       <c r="B87" s="31">
         <v>150</v>
       </c>
-      <c r="C87" s="162">
-        <f>$C$55*B87</f>
+      <c r="C87" s="107">
+        <f t="shared" si="1"/>
         <v>8.701918735891649</v>
       </c>
-      <c r="D87" s="162">
-        <f>$D$55*B87</f>
+      <c r="D87" s="107">
+        <f t="shared" si="2"/>
         <v>9.84326008307651</v>
       </c>
-      <c r="E87" s="170">
-        <f>$E$55*B87</f>
+      <c r="E87" s="112">
+        <f t="shared" si="3"/>
         <v>13.010869565217391</v>
       </c>
     </row>
@@ -7740,16 +7754,16 @@
       <c r="B88" s="31">
         <v>155</v>
       </c>
-      <c r="C88" s="162">
-        <f>$C$55*B88</f>
+      <c r="C88" s="107">
+        <f t="shared" si="1"/>
         <v>8.9919826937547036</v>
       </c>
-      <c r="D88" s="162">
-        <f>$D$55*B88</f>
+      <c r="D88" s="107">
+        <f t="shared" si="2"/>
         <v>10.171368752512395</v>
       </c>
-      <c r="E88" s="170">
-        <f>$E$55*B88</f>
+      <c r="E88" s="112">
+        <f t="shared" si="3"/>
         <v>13.444565217391304</v>
       </c>
     </row>
@@ -7757,16 +7771,16 @@
       <c r="B89" s="31">
         <v>160</v>
       </c>
-      <c r="C89" s="162">
-        <f>$C$55*B89</f>
+      <c r="C89" s="107">
+        <f t="shared" ref="C89:C120" si="4">$C$55*B89</f>
         <v>9.2820466516177582</v>
       </c>
-      <c r="D89" s="162">
-        <f>$D$55*B89</f>
+      <c r="D89" s="107">
+        <f t="shared" ref="D89:D120" si="5">$D$55*B89</f>
         <v>10.499477421948278</v>
       </c>
-      <c r="E89" s="170">
-        <f>$E$55*B89</f>
+      <c r="E89" s="112">
+        <f t="shared" ref="E89:E120" si="6">$E$55*B89</f>
         <v>13.878260869565217</v>
       </c>
     </row>
@@ -7774,16 +7788,16 @@
       <c r="B90" s="31">
         <v>165</v>
       </c>
-      <c r="C90" s="162">
-        <f>$C$55*B90</f>
+      <c r="C90" s="107">
+        <f t="shared" si="4"/>
         <v>9.5721106094808128</v>
       </c>
-      <c r="D90" s="162">
-        <f>$D$55*B90</f>
+      <c r="D90" s="107">
+        <f t="shared" si="5"/>
         <v>10.827586091384161</v>
       </c>
-      <c r="E90" s="170">
-        <f>$E$55*B90</f>
+      <c r="E90" s="112">
+        <f t="shared" si="6"/>
         <v>14.31195652173913</v>
       </c>
     </row>
@@ -7791,16 +7805,16 @@
       <c r="B91" s="31">
         <v>170</v>
       </c>
-      <c r="C91" s="162">
-        <f>$C$55*B91</f>
+      <c r="C91" s="107">
+        <f t="shared" si="4"/>
         <v>9.8621745673438674</v>
       </c>
-      <c r="D91" s="162">
-        <f>$D$55*B91</f>
+      <c r="D91" s="107">
+        <f t="shared" si="5"/>
         <v>11.155694760820046</v>
       </c>
-      <c r="E91" s="170">
-        <f>$E$55*B91</f>
+      <c r="E91" s="112">
+        <f t="shared" si="6"/>
         <v>14.745652173913044</v>
       </c>
     </row>
@@ -7808,16 +7822,16 @@
       <c r="B92" s="31">
         <v>175</v>
       </c>
-      <c r="C92" s="162">
-        <f>$C$55*B92</f>
+      <c r="C92" s="107">
+        <f t="shared" si="4"/>
         <v>10.152238525206922</v>
       </c>
-      <c r="D92" s="162">
-        <f>$D$55*B92</f>
+      <c r="D92" s="107">
+        <f t="shared" si="5"/>
         <v>11.483803430255929</v>
       </c>
-      <c r="E92" s="170">
-        <f>$E$55*B92</f>
+      <c r="E92" s="112">
+        <f t="shared" si="6"/>
         <v>15.179347826086957</v>
       </c>
     </row>
@@ -7825,16 +7839,16 @@
       <c r="B93" s="31">
         <v>180</v>
       </c>
-      <c r="C93" s="162">
-        <f>$C$55*B93</f>
+      <c r="C93" s="107">
+        <f t="shared" si="4"/>
         <v>10.442302483069978</v>
       </c>
-      <c r="D93" s="162">
-        <f>$D$55*B93</f>
+      <c r="D93" s="107">
+        <f t="shared" si="5"/>
         <v>11.811912099691813</v>
       </c>
-      <c r="E93" s="170">
-        <f>$E$55*B93</f>
+      <c r="E93" s="112">
+        <f t="shared" si="6"/>
         <v>15.61304347826087</v>
       </c>
     </row>
@@ -7842,16 +7856,16 @@
       <c r="B94" s="31">
         <v>185</v>
       </c>
-      <c r="C94" s="162">
-        <f>$C$55*B94</f>
+      <c r="C94" s="107">
+        <f t="shared" si="4"/>
         <v>10.732366440933033</v>
       </c>
-      <c r="D94" s="162">
-        <f>$D$55*B94</f>
+      <c r="D94" s="107">
+        <f t="shared" si="5"/>
         <v>12.140020769127696</v>
       </c>
-      <c r="E94" s="170">
-        <f>$E$55*B94</f>
+      <c r="E94" s="112">
+        <f t="shared" si="6"/>
         <v>16.046739130434784</v>
       </c>
     </row>
@@ -7859,16 +7873,16 @@
       <c r="B95" s="31">
         <v>190</v>
       </c>
-      <c r="C95" s="162">
-        <f>$C$55*B95</f>
+      <c r="C95" s="107">
+        <f t="shared" si="4"/>
         <v>11.022430398796088</v>
       </c>
-      <c r="D95" s="162">
-        <f>$D$55*B95</f>
+      <c r="D95" s="107">
+        <f t="shared" si="5"/>
         <v>12.468129438563579</v>
       </c>
-      <c r="E95" s="170">
-        <f>$E$55*B95</f>
+      <c r="E95" s="112">
+        <f t="shared" si="6"/>
         <v>16.480434782608697</v>
       </c>
     </row>
@@ -7876,16 +7890,16 @@
       <c r="B96" s="31">
         <v>195</v>
       </c>
-      <c r="C96" s="162">
-        <f>$C$55*B96</f>
+      <c r="C96" s="107">
+        <f t="shared" si="4"/>
         <v>11.312494356659142</v>
       </c>
-      <c r="D96" s="162">
-        <f>$D$55*B96</f>
+      <c r="D96" s="107">
+        <f t="shared" si="5"/>
         <v>12.796238107999464</v>
       </c>
-      <c r="E96" s="170">
-        <f>$E$55*B96</f>
+      <c r="E96" s="112">
+        <f t="shared" si="6"/>
         <v>16.91413043478261</v>
       </c>
     </row>
@@ -7893,16 +7907,16 @@
       <c r="B97" s="31">
         <v>200</v>
       </c>
-      <c r="C97" s="162">
-        <f>$C$55*B97</f>
+      <c r="C97" s="107">
+        <f t="shared" si="4"/>
         <v>11.602558314522197</v>
       </c>
-      <c r="D97" s="162">
-        <f>$D$55*B97</f>
+      <c r="D97" s="107">
+        <f t="shared" si="5"/>
         <v>13.124346777435347</v>
       </c>
-      <c r="E97" s="170">
-        <f>$E$55*B97</f>
+      <c r="E97" s="112">
+        <f t="shared" si="6"/>
         <v>17.347826086956523</v>
       </c>
     </row>
@@ -7910,16 +7924,16 @@
       <c r="B98" s="31">
         <v>205</v>
       </c>
-      <c r="C98" s="162">
-        <f>$C$55*B98</f>
+      <c r="C98" s="107">
+        <f t="shared" si="4"/>
         <v>11.892622272385253</v>
       </c>
-      <c r="D98" s="162">
-        <f>$D$55*B98</f>
+      <c r="D98" s="107">
+        <f t="shared" si="5"/>
         <v>13.45245544687123</v>
       </c>
-      <c r="E98" s="170">
-        <f>$E$55*B98</f>
+      <c r="E98" s="112">
+        <f t="shared" si="6"/>
         <v>17.781521739130437</v>
       </c>
     </row>
@@ -7927,16 +7941,16 @@
       <c r="B99" s="31">
         <v>210</v>
       </c>
-      <c r="C99" s="162">
-        <f>$C$55*B99</f>
+      <c r="C99" s="107">
+        <f t="shared" si="4"/>
         <v>12.182686230248308</v>
       </c>
-      <c r="D99" s="162">
-        <f>$D$55*B99</f>
+      <c r="D99" s="107">
+        <f t="shared" si="5"/>
         <v>13.780564116307115</v>
       </c>
-      <c r="E99" s="170">
-        <f>$E$55*B99</f>
+      <c r="E99" s="112">
+        <f t="shared" si="6"/>
         <v>18.21521739130435</v>
       </c>
     </row>
@@ -7944,16 +7958,16 @@
       <c r="B100" s="31">
         <v>215</v>
       </c>
-      <c r="C100" s="162">
-        <f>$C$55*B100</f>
+      <c r="C100" s="107">
+        <f t="shared" si="4"/>
         <v>12.472750188111362</v>
       </c>
-      <c r="D100" s="162">
-        <f>$D$55*B100</f>
+      <c r="D100" s="107">
+        <f t="shared" si="5"/>
         <v>14.108672785742998</v>
       </c>
-      <c r="E100" s="170">
-        <f>$E$55*B100</f>
+      <c r="E100" s="112">
+        <f t="shared" si="6"/>
         <v>18.64891304347826</v>
       </c>
     </row>
@@ -7961,16 +7975,16 @@
       <c r="B101" s="31">
         <v>220</v>
       </c>
-      <c r="C101" s="162">
-        <f>$C$55*B101</f>
+      <c r="C101" s="107">
+        <f t="shared" si="4"/>
         <v>12.762814145974417</v>
       </c>
-      <c r="D101" s="162">
-        <f>$D$55*B101</f>
+      <c r="D101" s="107">
+        <f t="shared" si="5"/>
         <v>14.436781455178881</v>
       </c>
-      <c r="E101" s="170">
-        <f>$E$55*B101</f>
+      <c r="E101" s="112">
+        <f t="shared" si="6"/>
         <v>19.082608695652173</v>
       </c>
     </row>
@@ -7978,16 +7992,16 @@
       <c r="B102" s="31">
         <v>225</v>
       </c>
-      <c r="C102" s="162">
-        <f>$C$55*B102</f>
+      <c r="C102" s="107">
+        <f t="shared" si="4"/>
         <v>13.052878103837472</v>
       </c>
-      <c r="D102" s="162">
-        <f>$D$55*B102</f>
+      <c r="D102" s="107">
+        <f t="shared" si="5"/>
         <v>14.764890124614766</v>
       </c>
-      <c r="E102" s="170">
-        <f>$E$55*B102</f>
+      <c r="E102" s="112">
+        <f t="shared" si="6"/>
         <v>19.516304347826086</v>
       </c>
     </row>
@@ -7995,16 +8009,16 @@
       <c r="B103" s="31">
         <v>230</v>
       </c>
-      <c r="C103" s="162">
-        <f>$C$55*B103</f>
+      <c r="C103" s="107">
+        <f t="shared" si="4"/>
         <v>13.342942061700526</v>
       </c>
-      <c r="D103" s="162">
-        <f>$D$55*B103</f>
+      <c r="D103" s="107">
+        <f t="shared" si="5"/>
         <v>15.092998794050649</v>
       </c>
-      <c r="E103" s="170">
-        <f>$E$55*B103</f>
+      <c r="E103" s="112">
+        <f t="shared" si="6"/>
         <v>19.95</v>
       </c>
     </row>
@@ -8012,16 +8026,16 @@
       <c r="B104" s="31">
         <v>235</v>
       </c>
-      <c r="C104" s="162">
-        <f>$C$55*B104</f>
+      <c r="C104" s="107">
+        <f t="shared" si="4"/>
         <v>13.633006019563583</v>
       </c>
-      <c r="D104" s="162">
-        <f>$D$55*B104</f>
+      <c r="D104" s="107">
+        <f t="shared" si="5"/>
         <v>15.421107463486534</v>
       </c>
-      <c r="E104" s="170">
-        <f>$E$55*B104</f>
+      <c r="E104" s="112">
+        <f t="shared" si="6"/>
         <v>20.383695652173913</v>
       </c>
     </row>
@@ -8029,16 +8043,16 @@
       <c r="B105" s="31">
         <v>240</v>
       </c>
-      <c r="C105" s="162">
-        <f>$C$55*B105</f>
+      <c r="C105" s="107">
+        <f t="shared" si="4"/>
         <v>13.923069977426637</v>
       </c>
-      <c r="D105" s="162">
-        <f>$D$55*B105</f>
+      <c r="D105" s="107">
+        <f t="shared" si="5"/>
         <v>15.749216132922417</v>
       </c>
-      <c r="E105" s="170">
-        <f>$E$55*B105</f>
+      <c r="E105" s="112">
+        <f t="shared" si="6"/>
         <v>20.817391304347826</v>
       </c>
     </row>
@@ -8046,16 +8060,16 @@
       <c r="B106" s="31">
         <v>245</v>
       </c>
-      <c r="C106" s="162">
-        <f>$C$55*B106</f>
+      <c r="C106" s="107">
+        <f t="shared" si="4"/>
         <v>14.213133935289692</v>
       </c>
-      <c r="D106" s="162">
-        <f>$D$55*B106</f>
+      <c r="D106" s="107">
+        <f t="shared" si="5"/>
         <v>16.077324802358302</v>
       </c>
-      <c r="E106" s="170">
-        <f>$E$55*B106</f>
+      <c r="E106" s="112">
+        <f t="shared" si="6"/>
         <v>21.251086956521739</v>
       </c>
     </row>
@@ -8063,16 +8077,16 @@
       <c r="B107" s="31">
         <v>250</v>
       </c>
-      <c r="C107" s="162">
-        <f>$C$55*B107</f>
+      <c r="C107" s="107">
+        <f t="shared" si="4"/>
         <v>14.503197893152747</v>
       </c>
-      <c r="D107" s="162">
-        <f>$D$55*B107</f>
+      <c r="D107" s="107">
+        <f t="shared" si="5"/>
         <v>16.405433471794183</v>
       </c>
-      <c r="E107" s="170">
-        <f>$E$55*B107</f>
+      <c r="E107" s="112">
+        <f t="shared" si="6"/>
         <v>21.684782608695652</v>
       </c>
     </row>
@@ -8080,16 +8094,16 @@
       <c r="B108" s="31">
         <v>255</v>
       </c>
-      <c r="C108" s="162">
-        <f>$C$55*B108</f>
+      <c r="C108" s="107">
+        <f t="shared" si="4"/>
         <v>14.793261851015801</v>
       </c>
-      <c r="D108" s="162">
-        <f>$D$55*B108</f>
+      <c r="D108" s="107">
+        <f t="shared" si="5"/>
         <v>16.733542141230068</v>
       </c>
-      <c r="E108" s="170">
-        <f>$E$55*B108</f>
+      <c r="E108" s="112">
+        <f t="shared" si="6"/>
         <v>22.118478260869566</v>
       </c>
     </row>
@@ -8097,16 +8111,16 @@
       <c r="B109" s="31">
         <v>260</v>
       </c>
-      <c r="C109" s="162">
-        <f>$C$55*B109</f>
+      <c r="C109" s="107">
+        <f t="shared" si="4"/>
         <v>15.083325808878858</v>
       </c>
-      <c r="D109" s="162">
-        <f>$D$55*B109</f>
+      <c r="D109" s="107">
+        <f t="shared" si="5"/>
         <v>17.061650810665952</v>
       </c>
-      <c r="E109" s="170">
-        <f>$E$55*B109</f>
+      <c r="E109" s="112">
+        <f t="shared" si="6"/>
         <v>22.552173913043479</v>
       </c>
     </row>
@@ -8114,16 +8128,16 @@
       <c r="B110" s="31">
         <v>265</v>
       </c>
-      <c r="C110" s="162">
-        <f>$C$55*B110</f>
+      <c r="C110" s="107">
+        <f t="shared" si="4"/>
         <v>15.373389766741912</v>
       </c>
-      <c r="D110" s="162">
-        <f>$D$55*B110</f>
+      <c r="D110" s="107">
+        <f t="shared" si="5"/>
         <v>17.389759480101834</v>
       </c>
-      <c r="E110" s="170">
-        <f>$E$55*B110</f>
+      <c r="E110" s="112">
+        <f t="shared" si="6"/>
         <v>22.985869565217392</v>
       </c>
     </row>
@@ -8131,16 +8145,16 @@
       <c r="B111" s="31">
         <v>270</v>
       </c>
-      <c r="C111" s="162">
-        <f>$C$55*B111</f>
+      <c r="C111" s="107">
+        <f t="shared" si="4"/>
         <v>15.663453724604967</v>
       </c>
-      <c r="D111" s="162">
-        <f>$D$55*B111</f>
+      <c r="D111" s="107">
+        <f t="shared" si="5"/>
         <v>17.717868149537718</v>
       </c>
-      <c r="E111" s="170">
-        <f>$E$55*B111</f>
+      <c r="E111" s="112">
+        <f t="shared" si="6"/>
         <v>23.419565217391305</v>
       </c>
     </row>
@@ -8148,16 +8162,16 @@
       <c r="B112" s="31">
         <v>275</v>
       </c>
-      <c r="C112" s="162">
-        <f>$C$55*B112</f>
+      <c r="C112" s="107">
+        <f t="shared" si="4"/>
         <v>15.953517682468021</v>
       </c>
-      <c r="D112" s="162">
-        <f>$D$55*B112</f>
+      <c r="D112" s="107">
+        <f t="shared" si="5"/>
         <v>18.045976818973603</v>
       </c>
-      <c r="E112" s="170">
-        <f>$E$55*B112</f>
+      <c r="E112" s="112">
+        <f t="shared" si="6"/>
         <v>23.853260869565219</v>
       </c>
     </row>
@@ -8165,16 +8179,16 @@
       <c r="B113" s="31">
         <v>280</v>
       </c>
-      <c r="C113" s="162">
-        <f>$C$55*B113</f>
+      <c r="C113" s="107">
+        <f t="shared" si="4"/>
         <v>16.243581640331076</v>
       </c>
-      <c r="D113" s="162">
-        <f>$D$55*B113</f>
+      <c r="D113" s="107">
+        <f t="shared" si="5"/>
         <v>18.374085488409484</v>
       </c>
-      <c r="E113" s="170">
-        <f>$E$55*B113</f>
+      <c r="E113" s="112">
+        <f t="shared" si="6"/>
         <v>24.286956521739132</v>
       </c>
     </row>
@@ -8182,16 +8196,16 @@
       <c r="B114" s="31">
         <v>285</v>
       </c>
-      <c r="C114" s="162">
-        <f>$C$55*B114</f>
+      <c r="C114" s="107">
+        <f t="shared" si="4"/>
         <v>16.533645598194131</v>
       </c>
-      <c r="D114" s="162">
-        <f>$D$55*B114</f>
+      <c r="D114" s="107">
+        <f t="shared" si="5"/>
         <v>18.702194157845369</v>
       </c>
-      <c r="E114" s="170">
-        <f>$E$55*B114</f>
+      <c r="E114" s="112">
+        <f t="shared" si="6"/>
         <v>24.720652173913045</v>
       </c>
     </row>
@@ -8199,16 +8213,16 @@
       <c r="B115" s="31">
         <v>290</v>
       </c>
-      <c r="C115" s="162">
-        <f>$C$55*B115</f>
+      <c r="C115" s="107">
+        <f t="shared" si="4"/>
         <v>16.823709556057185</v>
       </c>
-      <c r="D115" s="162">
-        <f>$D$55*B115</f>
+      <c r="D115" s="107">
+        <f t="shared" si="5"/>
         <v>19.030302827281254</v>
       </c>
-      <c r="E115" s="170">
-        <f>$E$55*B115</f>
+      <c r="E115" s="112">
+        <f t="shared" si="6"/>
         <v>25.154347826086958</v>
       </c>
     </row>
@@ -8216,16 +8230,16 @@
       <c r="B116" s="31">
         <v>295</v>
       </c>
-      <c r="C116" s="162">
-        <f>$C$55*B116</f>
+      <c r="C116" s="107">
+        <f t="shared" si="4"/>
         <v>17.11377351392024</v>
       </c>
-      <c r="D116" s="162">
-        <f>$D$55*B116</f>
+      <c r="D116" s="107">
+        <f t="shared" si="5"/>
         <v>19.358411496717139</v>
       </c>
-      <c r="E116" s="170">
-        <f>$E$55*B116</f>
+      <c r="E116" s="112">
+        <f t="shared" si="6"/>
         <v>25.588043478260872</v>
       </c>
     </row>
@@ -8233,16 +8247,16 @@
       <c r="B117" s="31">
         <v>300</v>
       </c>
-      <c r="C117" s="162">
-        <f>$C$55*B117</f>
+      <c r="C117" s="107">
+        <f t="shared" si="4"/>
         <v>17.403837471783298</v>
       </c>
-      <c r="D117" s="162">
-        <f>$D$55*B117</f>
+      <c r="D117" s="107">
+        <f t="shared" si="5"/>
         <v>19.68652016615302</v>
       </c>
-      <c r="E117" s="170">
-        <f>$E$55*B117</f>
+      <c r="E117" s="112">
+        <f t="shared" si="6"/>
         <v>26.021739130434781</v>
       </c>
     </row>
@@ -8250,16 +8264,16 @@
       <c r="B118" s="31">
         <v>305</v>
       </c>
-      <c r="C118" s="162">
-        <f>$C$55*B118</f>
+      <c r="C118" s="107">
+        <f t="shared" si="4"/>
         <v>17.693901429646353</v>
       </c>
-      <c r="D118" s="162">
-        <f>$D$55*B118</f>
+      <c r="D118" s="107">
+        <f t="shared" si="5"/>
         <v>20.014628835588905</v>
       </c>
-      <c r="E118" s="170">
-        <f>$E$55*B118</f>
+      <c r="E118" s="112">
+        <f t="shared" si="6"/>
         <v>26.455434782608695</v>
       </c>
     </row>
@@ -8267,16 +8281,16 @@
       <c r="B119" s="31">
         <v>310</v>
       </c>
-      <c r="C119" s="162">
-        <f>$C$55*B119</f>
+      <c r="C119" s="107">
+        <f t="shared" si="4"/>
         <v>17.983965387509407</v>
       </c>
-      <c r="D119" s="162">
-        <f>$D$55*B119</f>
+      <c r="D119" s="107">
+        <f t="shared" si="5"/>
         <v>20.34273750502479</v>
       </c>
-      <c r="E119" s="170">
-        <f>$E$55*B119</f>
+      <c r="E119" s="112">
+        <f t="shared" si="6"/>
         <v>26.889130434782608</v>
       </c>
     </row>
@@ -8284,16 +8298,16 @@
       <c r="B120" s="31">
         <v>315</v>
       </c>
-      <c r="C120" s="162">
-        <f>$C$55*B120</f>
+      <c r="C120" s="107">
+        <f t="shared" si="4"/>
         <v>18.274029345372462</v>
       </c>
-      <c r="D120" s="162">
-        <f>$D$55*B120</f>
+      <c r="D120" s="107">
+        <f t="shared" si="5"/>
         <v>20.670846174460671</v>
       </c>
-      <c r="E120" s="170">
-        <f>$E$55*B120</f>
+      <c r="E120" s="112">
+        <f t="shared" si="6"/>
         <v>27.322826086956521</v>
       </c>
     </row>
@@ -8301,16 +8315,16 @@
       <c r="B121" s="31">
         <v>320</v>
       </c>
-      <c r="C121" s="162">
-        <f>$C$55*B121</f>
+      <c r="C121" s="107">
+        <f t="shared" ref="C121:C152" si="7">$C$55*B121</f>
         <v>18.564093303235516</v>
       </c>
-      <c r="D121" s="162">
-        <f>$D$55*B121</f>
+      <c r="D121" s="107">
+        <f t="shared" ref="D121:D157" si="8">$D$55*B121</f>
         <v>20.998954843896556</v>
       </c>
-      <c r="E121" s="170">
-        <f>$E$55*B121</f>
+      <c r="E121" s="112">
+        <f t="shared" ref="E121:E157" si="9">$E$55*B121</f>
         <v>27.756521739130434</v>
       </c>
     </row>
@@ -8318,16 +8332,16 @@
       <c r="B122" s="31">
         <v>325</v>
       </c>
-      <c r="C122" s="162">
-        <f>$C$55*B122</f>
+      <c r="C122" s="107">
+        <f t="shared" si="7"/>
         <v>18.854157261098571</v>
       </c>
-      <c r="D122" s="162">
-        <f>$D$55*B122</f>
+      <c r="D122" s="107">
+        <f t="shared" si="8"/>
         <v>21.32706351333244</v>
       </c>
-      <c r="E122" s="170">
-        <f>$E$55*B122</f>
+      <c r="E122" s="112">
+        <f t="shared" si="9"/>
         <v>28.190217391304348</v>
       </c>
     </row>
@@ -8335,16 +8349,16 @@
       <c r="B123" s="31">
         <v>330</v>
       </c>
-      <c r="C123" s="162">
-        <f>$C$55*B123</f>
+      <c r="C123" s="107">
+        <f t="shared" si="7"/>
         <v>19.144221218961626</v>
       </c>
-      <c r="D123" s="162">
-        <f>$D$55*B123</f>
+      <c r="D123" s="107">
+        <f t="shared" si="8"/>
         <v>21.655172182768322</v>
       </c>
-      <c r="E123" s="170">
-        <f>$E$55*B123</f>
+      <c r="E123" s="112">
+        <f t="shared" si="9"/>
         <v>28.623913043478261</v>
       </c>
     </row>
@@ -8352,16 +8366,16 @@
       <c r="B124" s="31">
         <v>335</v>
       </c>
-      <c r="C124" s="162">
-        <f>$C$55*B124</f>
+      <c r="C124" s="107">
+        <f t="shared" si="7"/>
         <v>19.43428517682468</v>
       </c>
-      <c r="D124" s="162">
-        <f>$D$55*B124</f>
+      <c r="D124" s="107">
+        <f t="shared" si="8"/>
         <v>21.983280852204206</v>
       </c>
-      <c r="E124" s="170">
-        <f>$E$55*B124</f>
+      <c r="E124" s="112">
+        <f t="shared" si="9"/>
         <v>29.057608695652174</v>
       </c>
     </row>
@@ -8369,16 +8383,16 @@
       <c r="B125" s="31">
         <v>340</v>
       </c>
-      <c r="C125" s="162">
-        <f>$C$55*B125</f>
+      <c r="C125" s="107">
+        <f t="shared" si="7"/>
         <v>19.724349134687735</v>
       </c>
-      <c r="D125" s="162">
-        <f>$D$55*B125</f>
+      <c r="D125" s="107">
+        <f t="shared" si="8"/>
         <v>22.311389521640091</v>
       </c>
-      <c r="E125" s="170">
-        <f>$E$55*B125</f>
+      <c r="E125" s="112">
+        <f t="shared" si="9"/>
         <v>29.491304347826087</v>
       </c>
     </row>
@@ -8386,16 +8400,16 @@
       <c r="B126" s="31">
         <v>345</v>
       </c>
-      <c r="C126" s="162">
-        <f>$C$55*B126</f>
+      <c r="C126" s="107">
+        <f t="shared" si="7"/>
         <v>20.014413092550789</v>
       </c>
-      <c r="D126" s="162">
-        <f>$D$55*B126</f>
+      <c r="D126" s="107">
+        <f t="shared" si="8"/>
         <v>22.639498191075972</v>
       </c>
-      <c r="E126" s="170">
-        <f>$E$55*B126</f>
+      <c r="E126" s="112">
+        <f t="shared" si="9"/>
         <v>29.925000000000001</v>
       </c>
     </row>
@@ -8403,16 +8417,16 @@
       <c r="B127" s="31">
         <v>350</v>
       </c>
-      <c r="C127" s="162">
-        <f>$C$55*B127</f>
+      <c r="C127" s="107">
+        <f t="shared" si="7"/>
         <v>20.304477050413844</v>
       </c>
-      <c r="D127" s="162">
-        <f>$D$55*B127</f>
+      <c r="D127" s="107">
+        <f t="shared" si="8"/>
         <v>22.967606860511857</v>
       </c>
-      <c r="E127" s="170">
-        <f>$E$55*B127</f>
+      <c r="E127" s="112">
+        <f t="shared" si="9"/>
         <v>30.358695652173914</v>
       </c>
     </row>
@@ -8420,16 +8434,16 @@
       <c r="B128" s="31">
         <v>355</v>
       </c>
-      <c r="C128" s="162">
-        <f>$C$55*B128</f>
+      <c r="C128" s="107">
+        <f t="shared" si="7"/>
         <v>20.594541008276902</v>
       </c>
-      <c r="D128" s="162">
-        <f>$D$55*B128</f>
+      <c r="D128" s="107">
+        <f t="shared" si="8"/>
         <v>23.295715529947742</v>
       </c>
-      <c r="E128" s="170">
-        <f>$E$55*B128</f>
+      <c r="E128" s="112">
+        <f t="shared" si="9"/>
         <v>30.792391304347827</v>
       </c>
     </row>
@@ -8437,16 +8451,16 @@
       <c r="B129" s="31">
         <v>360</v>
       </c>
-      <c r="C129" s="162">
-        <f>$C$55*B129</f>
+      <c r="C129" s="107">
+        <f t="shared" si="7"/>
         <v>20.884604966139957</v>
       </c>
-      <c r="D129" s="162">
-        <f>$D$55*B129</f>
+      <c r="D129" s="107">
+        <f t="shared" si="8"/>
         <v>23.623824199383627</v>
       </c>
-      <c r="E129" s="170">
-        <f>$E$55*B129</f>
+      <c r="E129" s="112">
+        <f t="shared" si="9"/>
         <v>31.22608695652174</v>
       </c>
     </row>
@@ -8454,16 +8468,16 @@
       <c r="B130" s="31">
         <v>365</v>
       </c>
-      <c r="C130" s="162">
-        <f>$C$55*B130</f>
+      <c r="C130" s="107">
+        <f t="shared" si="7"/>
         <v>21.174668924003011</v>
       </c>
-      <c r="D130" s="162">
-        <f>$D$55*B130</f>
+      <c r="D130" s="107">
+        <f t="shared" si="8"/>
         <v>23.951932868819508</v>
       </c>
-      <c r="E130" s="170">
-        <f>$E$55*B130</f>
+      <c r="E130" s="112">
+        <f t="shared" si="9"/>
         <v>31.659782608695654</v>
       </c>
     </row>
@@ -8471,16 +8485,16 @@
       <c r="B131" s="31">
         <v>370</v>
       </c>
-      <c r="C131" s="162">
-        <f>$C$55*B131</f>
+      <c r="C131" s="107">
+        <f t="shared" si="7"/>
         <v>21.464732881866066</v>
       </c>
-      <c r="D131" s="162">
-        <f>$D$55*B131</f>
+      <c r="D131" s="107">
+        <f t="shared" si="8"/>
         <v>24.280041538255393</v>
       </c>
-      <c r="E131" s="170">
-        <f>$E$55*B131</f>
+      <c r="E131" s="112">
+        <f t="shared" si="9"/>
         <v>32.093478260869567</v>
       </c>
     </row>
@@ -8488,16 +8502,16 @@
       <c r="B132" s="31">
         <v>375</v>
       </c>
-      <c r="C132" s="162">
-        <f>$C$55*B132</f>
+      <c r="C132" s="107">
+        <f t="shared" si="7"/>
         <v>21.754796839729121</v>
       </c>
-      <c r="D132" s="162">
-        <f>$D$55*B132</f>
+      <c r="D132" s="107">
+        <f t="shared" si="8"/>
         <v>24.608150207691278</v>
       </c>
-      <c r="E132" s="170">
-        <f>$E$55*B132</f>
+      <c r="E132" s="112">
+        <f t="shared" si="9"/>
         <v>32.527173913043477</v>
       </c>
     </row>
@@ -8505,16 +8519,16 @@
       <c r="B133" s="31">
         <v>380</v>
       </c>
-      <c r="C133" s="162">
-        <f>$C$55*B133</f>
+      <c r="C133" s="107">
+        <f t="shared" si="7"/>
         <v>22.044860797592175</v>
       </c>
-      <c r="D133" s="162">
-        <f>$D$55*B133</f>
+      <c r="D133" s="107">
+        <f t="shared" si="8"/>
         <v>24.936258877127159</v>
       </c>
-      <c r="E133" s="170">
-        <f>$E$55*B133</f>
+      <c r="E133" s="112">
+        <f t="shared" si="9"/>
         <v>32.960869565217394</v>
       </c>
     </row>
@@ -8522,16 +8536,16 @@
       <c r="B134" s="31">
         <v>385</v>
       </c>
-      <c r="C134" s="162">
-        <f>$C$55*B134</f>
+      <c r="C134" s="107">
+        <f t="shared" si="7"/>
         <v>22.33492475545523</v>
       </c>
-      <c r="D134" s="162">
-        <f>$D$55*B134</f>
+      <c r="D134" s="107">
+        <f t="shared" si="8"/>
         <v>25.264367546563044</v>
       </c>
-      <c r="E134" s="170">
-        <f>$E$55*B134</f>
+      <c r="E134" s="112">
+        <f t="shared" si="9"/>
         <v>33.394565217391303</v>
       </c>
     </row>
@@ -8539,16 +8553,16 @@
       <c r="B135" s="31">
         <v>390</v>
       </c>
-      <c r="C135" s="162">
-        <f>$C$55*B135</f>
+      <c r="C135" s="107">
+        <f t="shared" si="7"/>
         <v>22.624988713318285</v>
       </c>
-      <c r="D135" s="162">
-        <f>$D$55*B135</f>
+      <c r="D135" s="107">
+        <f t="shared" si="8"/>
         <v>25.592476215998929</v>
       </c>
-      <c r="E135" s="170">
-        <f>$E$55*B135</f>
+      <c r="E135" s="112">
+        <f t="shared" si="9"/>
         <v>33.82826086956522</v>
       </c>
     </row>
@@ -8556,16 +8570,16 @@
       <c r="B136" s="31">
         <v>395</v>
       </c>
-      <c r="C136" s="162">
-        <f>$C$55*B136</f>
+      <c r="C136" s="107">
+        <f t="shared" si="7"/>
         <v>22.915052671181339</v>
       </c>
-      <c r="D136" s="162">
-        <f>$D$55*B136</f>
+      <c r="D136" s="107">
+        <f t="shared" si="8"/>
         <v>25.92058488543481</v>
       </c>
-      <c r="E136" s="170">
-        <f>$E$55*B136</f>
+      <c r="E136" s="112">
+        <f t="shared" si="9"/>
         <v>34.26195652173913</v>
       </c>
     </row>
@@ -8573,16 +8587,16 @@
       <c r="B137" s="31">
         <v>400</v>
       </c>
-      <c r="C137" s="162">
-        <f>$C$55*B137</f>
+      <c r="C137" s="107">
+        <f t="shared" si="7"/>
         <v>23.205116629044394</v>
       </c>
-      <c r="D137" s="162">
-        <f>$D$55*B137</f>
+      <c r="D137" s="107">
+        <f t="shared" si="8"/>
         <v>26.248693554870695</v>
       </c>
-      <c r="E137" s="170">
-        <f>$E$55*B137</f>
+      <c r="E137" s="112">
+        <f t="shared" si="9"/>
         <v>34.695652173913047</v>
       </c>
     </row>
@@ -8590,16 +8604,16 @@
       <c r="B138" s="31">
         <v>405</v>
       </c>
-      <c r="C138" s="162">
-        <f>$C$55*B138</f>
+      <c r="C138" s="107">
+        <f t="shared" si="7"/>
         <v>23.495180586907448</v>
       </c>
-      <c r="D138" s="162">
-        <f>$D$55*B138</f>
+      <c r="D138" s="107">
+        <f t="shared" si="8"/>
         <v>26.576802224306579</v>
       </c>
-      <c r="E138" s="170">
-        <f>$E$55*B138</f>
+      <c r="E138" s="112">
+        <f t="shared" si="9"/>
         <v>35.129347826086956</v>
       </c>
     </row>
@@ -8607,16 +8621,16 @@
       <c r="B139" s="31">
         <v>410</v>
       </c>
-      <c r="C139" s="162">
-        <f>$C$55*B139</f>
+      <c r="C139" s="107">
+        <f t="shared" si="7"/>
         <v>23.785244544770507</v>
       </c>
-      <c r="D139" s="162">
-        <f>$D$55*B139</f>
+      <c r="D139" s="107">
+        <f t="shared" si="8"/>
         <v>26.904910893742461</v>
       </c>
-      <c r="E139" s="170">
-        <f>$E$55*B139</f>
+      <c r="E139" s="112">
+        <f t="shared" si="9"/>
         <v>35.563043478260873</v>
       </c>
     </row>
@@ -8624,16 +8638,16 @@
       <c r="B140" s="31">
         <v>415</v>
       </c>
-      <c r="C140" s="162">
-        <f>$C$55*B140</f>
+      <c r="C140" s="107">
+        <f t="shared" si="7"/>
         <v>24.075308502633561</v>
       </c>
-      <c r="D140" s="162">
-        <f>$D$55*B140</f>
+      <c r="D140" s="107">
+        <f t="shared" si="8"/>
         <v>27.233019563178345</v>
       </c>
-      <c r="E140" s="170">
-        <f>$E$55*B140</f>
+      <c r="E140" s="112">
+        <f t="shared" si="9"/>
         <v>35.996739130434783</v>
       </c>
     </row>
@@ -8641,16 +8655,16 @@
       <c r="B141" s="31">
         <v>420</v>
       </c>
-      <c r="C141" s="162">
-        <f>$C$55*B141</f>
+      <c r="C141" s="107">
+        <f t="shared" si="7"/>
         <v>24.365372460496616</v>
       </c>
-      <c r="D141" s="162">
-        <f>$D$55*B141</f>
+      <c r="D141" s="107">
+        <f t="shared" si="8"/>
         <v>27.56112823261423</v>
       </c>
-      <c r="E141" s="170">
-        <f>$E$55*B141</f>
+      <c r="E141" s="112">
+        <f t="shared" si="9"/>
         <v>36.4304347826087</v>
       </c>
     </row>
@@ -8658,16 +8672,16 @@
       <c r="B142" s="31">
         <v>425</v>
       </c>
-      <c r="C142" s="162">
-        <f>$C$55*B142</f>
+      <c r="C142" s="107">
+        <f t="shared" si="7"/>
         <v>24.65543641835967</v>
       </c>
-      <c r="D142" s="162">
-        <f>$D$55*B142</f>
+      <c r="D142" s="107">
+        <f t="shared" si="8"/>
         <v>27.889236902050111</v>
       </c>
-      <c r="E142" s="170">
-        <f>$E$55*B142</f>
+      <c r="E142" s="112">
+        <f t="shared" si="9"/>
         <v>36.864130434782609</v>
       </c>
     </row>
@@ -8675,16 +8689,16 @@
       <c r="B143" s="31">
         <v>430</v>
       </c>
-      <c r="C143" s="162">
-        <f>$C$55*B143</f>
+      <c r="C143" s="107">
+        <f t="shared" si="7"/>
         <v>24.945500376222725</v>
       </c>
-      <c r="D143" s="162">
-        <f>$D$55*B143</f>
+      <c r="D143" s="107">
+        <f t="shared" si="8"/>
         <v>28.217345571485996</v>
       </c>
-      <c r="E143" s="170">
-        <f>$E$55*B143</f>
+      <c r="E143" s="112">
+        <f t="shared" si="9"/>
         <v>37.297826086956519</v>
       </c>
     </row>
@@ -8692,16 +8706,16 @@
       <c r="B144" s="31">
         <v>435</v>
       </c>
-      <c r="C144" s="162">
-        <f>$C$55*B144</f>
+      <c r="C144" s="107">
+        <f t="shared" si="7"/>
         <v>25.23556433408578</v>
       </c>
-      <c r="D144" s="162">
-        <f>$D$55*B144</f>
+      <c r="D144" s="107">
+        <f t="shared" si="8"/>
         <v>28.545454240921881</v>
       </c>
-      <c r="E144" s="170">
-        <f>$E$55*B144</f>
+      <c r="E144" s="112">
+        <f t="shared" si="9"/>
         <v>37.731521739130436</v>
       </c>
     </row>
@@ -8709,16 +8723,16 @@
       <c r="B145" s="31">
         <v>440</v>
       </c>
-      <c r="C145" s="162">
-        <f>$C$55*B145</f>
+      <c r="C145" s="107">
+        <f t="shared" si="7"/>
         <v>25.525628291948834</v>
       </c>
-      <c r="D145" s="162">
-        <f>$D$55*B145</f>
+      <c r="D145" s="107">
+        <f t="shared" si="8"/>
         <v>28.873562910357762</v>
       </c>
-      <c r="E145" s="170">
-        <f>$E$55*B145</f>
+      <c r="E145" s="112">
+        <f t="shared" si="9"/>
         <v>38.165217391304346</v>
       </c>
     </row>
@@ -8726,16 +8740,16 @@
       <c r="B146" s="31">
         <v>445</v>
       </c>
-      <c r="C146" s="162">
-        <f>$C$55*B146</f>
+      <c r="C146" s="107">
+        <f t="shared" si="7"/>
         <v>25.815692249811889</v>
       </c>
-      <c r="D146" s="162">
-        <f>$D$55*B146</f>
+      <c r="D146" s="107">
+        <f t="shared" si="8"/>
         <v>29.201671579793647</v>
       </c>
-      <c r="E146" s="170">
-        <f>$E$55*B146</f>
+      <c r="E146" s="112">
+        <f t="shared" si="9"/>
         <v>38.598913043478262</v>
       </c>
     </row>
@@ -8743,16 +8757,16 @@
       <c r="B147" s="31">
         <v>450</v>
       </c>
-      <c r="C147" s="162">
-        <f>$C$55*B147</f>
+      <c r="C147" s="107">
+        <f t="shared" si="7"/>
         <v>26.105756207674943</v>
       </c>
-      <c r="D147" s="162">
-        <f>$D$55*B147</f>
+      <c r="D147" s="107">
+        <f t="shared" si="8"/>
         <v>29.529780249229532</v>
       </c>
-      <c r="E147" s="170">
-        <f>$E$55*B147</f>
+      <c r="E147" s="112">
+        <f t="shared" si="9"/>
         <v>39.032608695652172</v>
       </c>
     </row>
@@ -8760,16 +8774,16 @@
       <c r="B148" s="31">
         <v>455</v>
       </c>
-      <c r="C148" s="162">
-        <f>$C$55*B148</f>
+      <c r="C148" s="107">
+        <f t="shared" si="7"/>
         <v>26.395820165537998</v>
       </c>
-      <c r="D148" s="162">
-        <f>$D$55*B148</f>
+      <c r="D148" s="107">
+        <f t="shared" si="8"/>
         <v>29.857888918665417</v>
       </c>
-      <c r="E148" s="170">
-        <f>$E$55*B148</f>
+      <c r="E148" s="112">
+        <f t="shared" si="9"/>
         <v>39.466304347826089</v>
       </c>
     </row>
@@ -8777,16 +8791,16 @@
       <c r="B149" s="31">
         <v>460</v>
       </c>
-      <c r="C149" s="162">
-        <f>$C$55*B149</f>
+      <c r="C149" s="107">
+        <f t="shared" si="7"/>
         <v>26.685884123401053</v>
       </c>
-      <c r="D149" s="162">
-        <f>$D$55*B149</f>
+      <c r="D149" s="107">
+        <f t="shared" si="8"/>
         <v>30.185997588101298</v>
       </c>
-      <c r="E149" s="170">
-        <f>$E$55*B149</f>
+      <c r="E149" s="112">
+        <f t="shared" si="9"/>
         <v>39.9</v>
       </c>
     </row>
@@ -8794,16 +8808,16 @@
       <c r="B150" s="31">
         <v>465</v>
       </c>
-      <c r="C150" s="162">
-        <f>$C$55*B150</f>
+      <c r="C150" s="107">
+        <f t="shared" si="7"/>
         <v>26.975948081264111</v>
       </c>
-      <c r="D150" s="162">
-        <f>$D$55*B150</f>
+      <c r="D150" s="107">
+        <f t="shared" si="8"/>
         <v>30.514106257537183</v>
       </c>
-      <c r="E150" s="170">
-        <f>$E$55*B150</f>
+      <c r="E150" s="112">
+        <f t="shared" si="9"/>
         <v>40.333695652173915</v>
       </c>
     </row>
@@ -8811,16 +8825,16 @@
       <c r="B151" s="31">
         <v>470</v>
       </c>
-      <c r="C151" s="162">
-        <f>$C$55*B151</f>
+      <c r="C151" s="107">
+        <f t="shared" si="7"/>
         <v>27.266012039127165</v>
       </c>
-      <c r="D151" s="162">
-        <f>$D$55*B151</f>
+      <c r="D151" s="107">
+        <f t="shared" si="8"/>
         <v>30.842214926973067</v>
       </c>
-      <c r="E151" s="170">
-        <f>$E$55*B151</f>
+      <c r="E151" s="112">
+        <f t="shared" si="9"/>
         <v>40.767391304347825</v>
       </c>
     </row>
@@ -8828,16 +8842,16 @@
       <c r="B152" s="31">
         <v>475</v>
       </c>
-      <c r="C152" s="162">
-        <f>$C$55*B152</f>
+      <c r="C152" s="107">
+        <f t="shared" si="7"/>
         <v>27.55607599699022</v>
       </c>
-      <c r="D152" s="162">
-        <f>$D$55*B152</f>
+      <c r="D152" s="107">
+        <f t="shared" si="8"/>
         <v>31.170323596408949</v>
       </c>
-      <c r="E152" s="170">
-        <f>$E$55*B152</f>
+      <c r="E152" s="112">
+        <f t="shared" si="9"/>
         <v>41.201086956521742</v>
       </c>
     </row>
@@ -8845,16 +8859,16 @@
       <c r="B153" s="31">
         <v>480</v>
       </c>
-      <c r="C153" s="162">
-        <f>$C$55*B153</f>
+      <c r="C153" s="107">
+        <f t="shared" ref="C153:C184" si="10">$C$55*B153</f>
         <v>27.846139954853275</v>
       </c>
-      <c r="D153" s="162">
-        <f>$D$55*B153</f>
+      <c r="D153" s="107">
+        <f t="shared" si="8"/>
         <v>31.498432265844833</v>
       </c>
-      <c r="E153" s="170">
-        <f>$E$55*B153</f>
+      <c r="E153" s="112">
+        <f t="shared" si="9"/>
         <v>41.634782608695652</v>
       </c>
     </row>
@@ -8862,16 +8876,16 @@
       <c r="B154" s="31">
         <v>485</v>
       </c>
-      <c r="C154" s="162">
-        <f>$C$55*B154</f>
+      <c r="C154" s="107">
+        <f t="shared" si="10"/>
         <v>28.136203912716329</v>
       </c>
-      <c r="D154" s="162">
-        <f>$D$55*B154</f>
+      <c r="D154" s="107">
+        <f t="shared" si="8"/>
         <v>31.826540935280718</v>
       </c>
-      <c r="E154" s="170">
-        <f>$E$55*B154</f>
+      <c r="E154" s="112">
+        <f t="shared" si="9"/>
         <v>42.068478260869568</v>
       </c>
     </row>
@@ -8879,16 +8893,16 @@
       <c r="B155" s="31">
         <v>490</v>
       </c>
-      <c r="C155" s="162">
-        <f>$C$55*B155</f>
+      <c r="C155" s="107">
+        <f t="shared" si="10"/>
         <v>28.426267870579384</v>
       </c>
-      <c r="D155" s="162">
-        <f>$D$55*B155</f>
+      <c r="D155" s="107">
+        <f t="shared" si="8"/>
         <v>32.154649604716603</v>
       </c>
-      <c r="E155" s="170">
-        <f>$E$55*B155</f>
+      <c r="E155" s="112">
+        <f t="shared" si="9"/>
         <v>42.502173913043478</v>
       </c>
     </row>
@@ -8896,16 +8910,16 @@
       <c r="B156" s="31">
         <v>495</v>
       </c>
-      <c r="C156" s="162">
-        <f>$C$55*B156</f>
+      <c r="C156" s="107">
+        <f t="shared" si="10"/>
         <v>28.716331828442438</v>
       </c>
-      <c r="D156" s="162">
-        <f>$D$55*B156</f>
+      <c r="D156" s="107">
+        <f t="shared" si="8"/>
         <v>32.482758274152488</v>
       </c>
-      <c r="E156" s="170">
-        <f>$E$55*B156</f>
+      <c r="E156" s="112">
+        <f t="shared" si="9"/>
         <v>42.935869565217395</v>
       </c>
     </row>
@@ -8913,21 +8927,22 @@
       <c r="B157" s="32">
         <v>500</v>
       </c>
-      <c r="C157" s="171">
-        <f>$C$55*B157</f>
+      <c r="C157" s="113">
+        <f t="shared" si="10"/>
         <v>29.006395786305493</v>
       </c>
-      <c r="D157" s="171">
-        <f>$D$55*B157</f>
+      <c r="D157" s="113">
+        <f t="shared" si="8"/>
         <v>32.810866943588366</v>
       </c>
-      <c r="E157" s="172">
-        <f>$E$55*B157</f>
+      <c r="E157" s="114">
+        <f t="shared" si="9"/>
         <v>43.369565217391305</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="A52:E52"/>
     <mergeCell ref="B56:E56"/>
     <mergeCell ref="A35:D35"/>
@@ -8936,7 +8951,6 @@
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="J24:K24"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8945,10 +8959,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACC50A1-9512-4A2C-8EB9-0AAA8B7135B9}">
-  <dimension ref="D1:J15"/>
+  <dimension ref="D1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8959,14 +8973,14 @@
     <col min="9" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="I2" s="135" t="s">
+    <row r="1" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="178" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="136"/>
-    </row>
-    <row r="3" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="179"/>
+    </row>
+    <row r="3" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="32" t="s">
         <v>112</v>
       </c>
@@ -8974,14 +8988,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I5" s="137" t="s">
+    <row r="4" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="180" t="s">
         <v>114</v>
       </c>
-      <c r="J5" s="138"/>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="181"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="I6" s="87" t="s">
         <v>115</v>
       </c>
@@ -8989,24 +9003,27 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="I7" s="88" t="s">
         <v>116</v>
       </c>
       <c r="J7" s="90">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.44440000000000002</v>
+      </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I8" s="92" t="s">
         <v>117</v>
       </c>
       <c r="J8" s="91">
         <f>J7/J6</f>
-        <v>0.66666666666666674</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+        <v>0.7406666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="86"/>
     </row>
   </sheetData>

</xml_diff>